<commit_message>
Documentation: Final GANTT updates
</commit_message>
<xml_diff>
--- a/2_Documentation/2_Project_Planning/GANTT/GANTT.xlsx
+++ b/2_Documentation/2_Project_Planning/GANTT/GANTT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="248" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FBB7A3E-05FC-4C68-9BFF-E6CDEE9E12D1}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9C9CDBE-B0FF-494F-8F26-0436D8058229}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3525" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -892,10 +892,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1129,7 +1125,7 @@
   </sheetPr>
   <dimension ref="B1:AL25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -1474,13 +1470,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="22">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F9" s="22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
@@ -1550,13 +1546,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="22">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F11" s="22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G11" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -1588,13 +1584,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="22">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F12" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
@@ -1664,13 +1660,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="22">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F14" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
@@ -1702,13 +1698,13 @@
         <v>3</v>
       </c>
       <c r="E15" s="22">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F15" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
@@ -1740,13 +1736,13 @@
         <v>3</v>
       </c>
       <c r="E16" s="22">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F16" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
@@ -1778,13 +1774,13 @@
         <v>3</v>
       </c>
       <c r="E17" s="22">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F17" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
@@ -1816,13 +1812,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="22">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="F18" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
@@ -1886,7 +1882,7 @@
         <v>14</v>
       </c>
       <c r="G20" s="25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
@@ -1921,10 +1917,10 @@
         <v>42</v>
       </c>
       <c r="F21" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G21" s="25">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
@@ -1962,7 +1958,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
@@ -1994,13 +1990,13 @@
         <v>1</v>
       </c>
       <c r="E23" s="22">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="F23" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
@@ -2070,13 +2066,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="28">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F25" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>

</xml_diff>